<commit_message>
Update main.py to support new cashflow forecasting features
</commit_message>
<xml_diff>
--- a/sample_cf.xlsx
+++ b/sample_cf.xlsx
@@ -1,38 +1,82 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nulak2050\PycharmProjects\project_cf_ai_agent\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4559BB4C-F208-4831-A6EE-E3DBCCED39C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="As-Sold" sheetId="1" r:id="rId1"/>
+    <sheet name="Actual" sheetId="2" r:id="rId2"/>
+    <sheet name="VO" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Planned</t>
-  </si>
-  <si>
-    <t>Actual</t>
+    <t>Planned Inflow</t>
+  </si>
+  <si>
+    <t>Planned Outflow</t>
+  </si>
+  <si>
+    <t>Planned Net</t>
+  </si>
+  <si>
+    <t>Planned Value (PV)</t>
+  </si>
+  <si>
+    <t>Actual Inflow</t>
+  </si>
+  <si>
+    <t>Actual Outflow</t>
+  </si>
+  <si>
+    <t>Actual Net</t>
+  </si>
+  <si>
+    <t>Actual Cost (AC)</t>
+  </si>
+  <si>
+    <t>Earned Value (EV)</t>
+  </si>
+  <si>
+    <t>VO Amount</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Scope increase</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Additional resources</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,13 +140,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -140,7 +192,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -174,6 +226,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -208,9 +261,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -383,14 +437,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,137 +456,323 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>45658</v>
+        <v>45292</v>
       </c>
       <c r="B2">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="C2">
-        <v>9500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>80000</v>
+      </c>
+      <c r="D2">
+        <v>20000</v>
+      </c>
+      <c r="E2">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>45689</v>
+        <v>45323</v>
       </c>
       <c r="B3">
-        <v>11000</v>
+        <v>120000</v>
       </c>
       <c r="C3">
-        <v>10450</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>85000</v>
+      </c>
+      <c r="D3">
+        <v>35000</v>
+      </c>
+      <c r="E3">
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>45717</v>
+        <v>45352</v>
       </c>
       <c r="B4">
-        <v>12000</v>
+        <v>110000</v>
       </c>
       <c r="C4">
-        <v>11400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>90000</v>
+      </c>
+      <c r="D4">
+        <v>20000</v>
+      </c>
+      <c r="E4">
+        <v>97000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>45748</v>
+        <v>45383</v>
       </c>
       <c r="B5">
-        <v>13000</v>
+        <v>115000</v>
       </c>
       <c r="C5">
-        <v>12350</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>87000</v>
+      </c>
+      <c r="D5">
+        <v>28000</v>
+      </c>
+      <c r="E5">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>45778</v>
+        <v>45413</v>
       </c>
       <c r="B6">
-        <v>14000</v>
+        <v>130000</v>
       </c>
       <c r="C6">
-        <v>13300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>95000</v>
+      </c>
+      <c r="D6">
+        <v>35000</v>
+      </c>
+      <c r="E6">
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>45809</v>
+        <v>45444</v>
       </c>
       <c r="B7">
-        <v>15000</v>
+        <v>125000</v>
       </c>
       <c r="C7">
-        <v>14250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2">
-        <v>45839</v>
-      </c>
-      <c r="B8">
+        <v>92000</v>
+      </c>
+      <c r="D7">
+        <v>33000</v>
+      </c>
+      <c r="E7">
+        <v>115000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45292</v>
+      </c>
+      <c r="B2">
+        <v>98000</v>
+      </c>
+      <c r="C2">
+        <v>82000</v>
+      </c>
+      <c r="D2">
         <v>16000</v>
       </c>
-      <c r="C8">
-        <v>15200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2">
-        <v>45870</v>
-      </c>
-      <c r="B9">
-        <v>17000</v>
-      </c>
-      <c r="C9">
-        <v>16150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2">
-        <v>45901</v>
-      </c>
-      <c r="B10">
-        <v>18000</v>
-      </c>
-      <c r="C10">
-        <v>17100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2">
-        <v>45931</v>
-      </c>
-      <c r="B11">
-        <v>19000</v>
-      </c>
-      <c r="C11">
-        <v>18050</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2">
-        <v>45962</v>
-      </c>
-      <c r="B12">
-        <v>20000</v>
-      </c>
-      <c r="C12">
-        <v>19000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2">
-        <v>45992</v>
-      </c>
-      <c r="B13">
-        <v>21000</v>
-      </c>
-      <c r="C13">
-        <v>19950</v>
+      <c r="E2">
+        <v>85000</v>
+      </c>
+      <c r="F2">
+        <v>87000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>45323</v>
+      </c>
+      <c r="B3">
+        <v>118000</v>
+      </c>
+      <c r="C3">
+        <v>88000</v>
+      </c>
+      <c r="D3">
+        <v>30000</v>
+      </c>
+      <c r="E3">
+        <v>87000</v>
+      </c>
+      <c r="F3">
+        <v>88000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>45352</v>
+      </c>
+      <c r="B4">
+        <v>108000</v>
+      </c>
+      <c r="C4">
+        <v>92000</v>
+      </c>
+      <c r="D4">
+        <v>16000</v>
+      </c>
+      <c r="E4">
+        <v>88000</v>
+      </c>
+      <c r="F4">
+        <v>89000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>45383</v>
+      </c>
+      <c r="B5">
+        <v>113000</v>
+      </c>
+      <c r="C5">
+        <v>89000</v>
+      </c>
+      <c r="D5">
+        <v>24000</v>
+      </c>
+      <c r="E5">
+        <v>91000</v>
+      </c>
+      <c r="F5">
+        <v>93000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>45413</v>
+      </c>
+      <c r="B6">
+        <v>128000</v>
+      </c>
+      <c r="C6">
+        <v>97000</v>
+      </c>
+      <c r="D6">
+        <v>31000</v>
+      </c>
+      <c r="E6">
+        <v>94000</v>
+      </c>
+      <c r="F6">
+        <v>96000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>45444</v>
+      </c>
+      <c r="B7">
+        <v>123000</v>
+      </c>
+      <c r="C7">
+        <v>94000</v>
+      </c>
+      <c r="D7">
+        <v>29000</v>
+      </c>
+      <c r="E7">
+        <v>95000</v>
+      </c>
+      <c r="F7">
+        <v>98000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45292</v>
+      </c>
+      <c r="B2">
+        <v>5000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>45352</v>
+      </c>
+      <c r="B3">
+        <v>-3000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>45413</v>
+      </c>
+      <c r="B4">
+        <v>7000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>